<commit_message>
add excel test data
</commit_message>
<xml_diff>
--- a/testdata/excel2json/new_excel2json_files/lists/list3.xlsx
+++ b/testdata/excel2json/new_excel2json_files/lists/list3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/new_excel2json_files/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B48248-1ECE-F741-89A6-7410CF03C6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29636C0-8898-DC4B-9D77-91FB4F898D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1020" windowWidth="20280" windowHeight="20060" xr2:uid="{6E47428F-2F66-AC4F-A856-3DFB087A3678}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>ID (optional)</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Node 4</t>
+  </si>
+  <si>
+    <t>en_comments</t>
   </si>
 </sst>
 </file>
@@ -436,96 +439,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536F90FD-E3BA-C247-B844-CE7390669479}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1">
+  <conditionalFormatting sqref="A1:B1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>